<commit_message>
Assignment 2 extra files added and worked on
</commit_message>
<xml_diff>
--- a/Normalisation.xlsx
+++ b/Normalisation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CBAA0CB0-8A83-4D47-8183-0F06DB4CE835}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9842040C-194C-4A72-996A-DDE1A6072EF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1NF - 2NF" sheetId="1" r:id="rId1"/>
@@ -6064,8 +6064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FB8B18-5857-4843-AAF4-C59A18A2B916}">
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6865,8 +6865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B253C-8CC3-491C-96AE-B8AC45EAD542}">
   <dimension ref="B1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6919,11 +6919,11 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">

</xml_diff>